<commit_message>
added codes for capturing bivariate interactions
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/model_log.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/model_log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7104" yWindow="0" windowWidth="18312" windowHeight="7224" activeTab="3"/>
+    <workbookView xWindow="7992" yWindow="0" windowWidth="18312" windowHeight="7224" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="172">
   <si>
     <t>Model</t>
   </si>
@@ -270,6 +270,282 @@
   </si>
   <si>
     <t>2017-08-04 10:58:40.708023 Training XGBoost classifier, [0.6, 5, 1, 0.6]</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:44:39.312890 Reading Data</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:51:41.992507 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:52:16.764041 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:52:29.360894 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.974210446955,[[285360, 9909], [5313, 289657]],0.996756869374</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:52:34.369438 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.973900491494,[[94894, 3330], [1805, 96718]],0.996664464957</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:52:45.904398 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.955227508092,[[1125304, 44756], [9588, 34133]],0.942214761848</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:53:24.251243 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:53:35.556162 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.974054577891,[[285401, 9911], [5403, 289524]],0.996734039175</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:53:40.160091 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.973717515388,[[94866, 3315], [1856, 96710]],0.996662036642</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:53:51.602596 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.955256343607,[[1125334, 44726], [9583, 34138]],0.943048285685</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:54:29.380907 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:54:40.777876 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.974159663866,[[284998, 9898], [5354, 289990]],0.996749526811</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:54:45.438674 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.974159576307,[[95300, 3297], [1787, 96362]],0.996645251134</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:54:57.006097 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.955323077227,[[1125438, 44622], [9606, 34115]],0.94306868085</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:55:33.341078 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:55:44.647532 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.974259623204,[[285232, 9770], [5423, 289815]],0.996761222941</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:55:49.201041 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.973285352688,[[95141, 3350], [1906, 96349]],0.996564106931</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:56:00.425605 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.955674870508,[[1125886, 44174], [9627, 34094]],0.941991886331</t>
+  </si>
+  <si>
+    <t>bivariate countrycode X [merchant, offer, site, category] added</t>
+  </si>
+  <si>
+    <t>2017-08-04 23:51:41.993496 Training XGBoost classifier, [0.6, 5, 1, 0.6]</t>
+  </si>
+  <si>
+    <t>&lt;type 'generator'&gt;</t>
+  </si>
+  <si>
+    <t>0,Train1,Train2,0.985681208872,0.970740966714,[[131930, 1068], [1047, 13663]],[[153458, 8919], [4029, 276124]],0.99785688573,0.995317911718,0.97447978612,[[285388, 9987], [5076, 289787]],0.99686906934</t>
+  </si>
+  <si>
+    <t>0,Test1,Test2,0.984544143632,0.970449661381,[[43907, 407], [354, 4569]],[[50774, 3030], [1329, 92378]],0.997371416735,0.99514034294,0.973976863805,[[94681, 3437], [1683, 96947]],0.996685112499</t>
+  </si>
+  <si>
+    <t>1,Train1,Train2,0.985478203766,0.97091729167,[[131884, 1106], [1039, 13680]],[[153478, 8770], [4100, 276183]],0.997797346119,0.995339483529,0.974561195446,[[285362, 9876], [5139, 289863]],0.996868536973</t>
+  </si>
+  <si>
+    <t>1,Test1,Test2,0.98466569177,0.969608840079,[[43926, 396], [359, 4555]],[[50908, 3025], [1458, 92119]],0.997512269471,0.994906581192,0.973376841206,[[94834, 3421], [1817, 96674]],0.996578824515</t>
+  </si>
+  <si>
+    <t>2,Train1,Train2,0.985803167038,0.970887915197,[[131938, 1066], [1031, 13674]],[[153403, 8754], [4129, 276245]],0.997904108766,0.995318463705,0.974620493359,[[285341, 9820], [5160, 289919]],0.996876220911</t>
+  </si>
+  <si>
+    <t>2,Test1,Test2,0.983629864327,0.970747745916,[[43912, 396], [410, 4518]],[[51136, 2888], [1427, 92059]],0.997205211853,0.99521315839,0.973971516575,[[95048, 3284], [1837, 96577]],0.996705586608</t>
+  </si>
+  <si>
+    <t>3,Train1,Train2,0.98527510172,0.970788487134,[[131847, 1097], [1078, 13687]],[[152941, 8820], [4107, 276663]],0.997755757937,0.99527652193,0.974413797777,[[284788, 9917], [5185, 290350]],0.996831616874</t>
+  </si>
+  <si>
+    <t>3,Test1,Test2,0.984889105533,0.970463019456,[[44002, 366], [378, 4490]],[[51455, 2965], [1392, 91698]],0.997614865574,0.995216639389,0.974073170484,[[95457, 3331], [1770, 96188]],0.996759522448</t>
+  </si>
+  <si>
+    <t>Using two models, one for counry b and one for others</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:34:57.424100 Training XGBoost classifier, [0.6, 5, 1, 0.6]</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:35:34.820163 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:35:46.036633 KF_Index,Train1,Train2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:35:50.561203 KF_Index,Test1,Test2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:36:02.535875 KF_Index,Unseen1,Unseen2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>0,Unseen1,Unseen2,0.987117265479,0.929412416302,[[520019, 5446], [1352, 866]],[[604386, 40209], [8221, 33282]],0.850048703052,0.939074674047,0.954499205376,[[1124405, 45655], [9573, 34148]],0.94510049037</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:36:41.600096 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:36:51.524299 KF_Index,Train1,Train2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:36:55.633960 KF_Index,Test1,Test2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:37:07.426286 KF_Index,Unseen1,Unseen2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>1,Unseen1,Unseen2,0.987100209785,0.929772423182,[[520018, 5447], [1360, 858]],[[604639, 39956], [8227, 33276]],0.852429185119,0.938243844459,0.954695286876,[[1124657, 45403], [9587, 34134]],0.944835934651</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:37:45.449663 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:37:55.368839 KF_Index,Train1,Train2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:37:59.471749 KF_Index,Test1,Test2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:38:11.242442 KF_Index,Unseen1,Unseen2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2,Unseen1,Unseen2,0.987094524554,0.930437051267,[[520008, 5457], [1353, 865]],[[605100, 39495], [8232, 33271]],0.853204505105,0.937976678464,0.955068500825,[[1125108, 44952], [9585, 34136]],0.944313517651</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:38:49.749662 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:38:59.588111 KF_Index,Train1,Train2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:39:05.471325 KF_Index,Test1,Test2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:39:18.012937 KF_Index,Unseen1,Unseen2,Accuracy1,Accuracy2,CM1,CM2,AUC1,AUC2,Accuracy12,CM12,AUC12</t>
+  </si>
+  <si>
+    <t>3,Unseen1,Unseen2,0.987263186421,0.929722867579,[[520100, 5365], [1356, 862]],[[604605, 39990], [8227, 33276]],0.853677957117,0.936925994516,0.954738128213,[[1124705, 45355], [9583, 34138]],0.94297465591</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:48:40.516418 Training Random Forest classifier, [5, 2, 5, 120]</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:49:56.816046 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:50:15.738101 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.964517763143,[[282377, 12892], [8051, 286919]],0.993280837568</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:50:22.746739 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.964055360438,[[93917, 4307], [2765, 95758]],0.993183844751</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:50:54.716999 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.94615420739,[[1111160, 58900], [6457, 37264]],0.975016533199</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:52:02.302387 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:52:20.081917 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.964417803635,[[282582, 12730], [8272, 286655]],0.993337909365</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:52:27.070110 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.964650032783,[[93999, 4182], [2773, 95793]],0.993277102165</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:52:58.910701 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.946959130189,[[1112116, 57944], [6436, 37285]],0.975065253311</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:54:24.010453 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:54:41.832144 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.965349688262,[[282496, 12400], [8052, 287292]],0.993411147791</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:54:48.835470 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.965666392201,[[94481, 4116], [2639, 95510]],0.993608764263</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:55:20.805254 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.947712149061,[[1113671, 56389], [7077, 36644]],0.973882304881</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:56:37.320759 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:56:55.156944 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.965024396856,[[282582, 12420], [8224, 287014]],0.993371558607</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:57:02.183943 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.964497372246,[[94259, 4232], [2753, 95502]],0.993192841218</t>
+  </si>
+  <si>
+    <t>2017-08-05 02:57:34.072687 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.947572914719,[[1112956, 57104], [6531, 37190]],0.975265871796</t>
   </si>
 </sst>
 </file>
@@ -10817,289 +11093,700 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A2:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J19" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J25" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J25" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="J30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J30" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="J31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J31" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="J32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J32" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="J33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J33" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="J34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J34" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="J35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J35" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="J36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J36" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="J37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J37" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>151</v>
+      </c>
+      <c r="J39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J39" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="J40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J40" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="J41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J41" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="J42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J42" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J43" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="J44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J44" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>157</v>
+      </c>
+      <c r="J45" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>161</v>
+      </c>
+      <c r="J49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>162</v>
+      </c>
+      <c r="J50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>163</v>
+      </c>
+      <c r="J51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="J52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>165</v>
+      </c>
+      <c r="J53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>166</v>
+      </c>
+      <c r="J54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>167</v>
+      </c>
+      <c r="J55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>168</v>
+      </c>
+      <c r="J56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>169</v>
+      </c>
+      <c r="J57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>170</v>
+      </c>
+      <c r="J58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>171</v>
+      </c>
+      <c r="J59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J75" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J78" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J87" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J88" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J91" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J92" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J93" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J94" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J95" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J96" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J97" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J98" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J99" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J100" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="101" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J101" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J102" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J103" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="104" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J104" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J105" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J106" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J107" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J108" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J109" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="110" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J110" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J111" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J112" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J113" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added code for creating unseen dataset based on date and also calculated the correlation coefficients
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/model_log.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/model_log.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7992" yWindow="0" windowWidth="18312" windowHeight="7224" activeTab="3"/>
+    <workbookView xWindow="8880" yWindow="0" windowWidth="18312" windowHeight="7224" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$W$4:$Y$220</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="477">
   <si>
     <t>Model</t>
   </si>
@@ -546,6 +547,921 @@
   </si>
   <si>
     <t>3,Unseen,0.947572914719,[[1112956, 57104], [6531, 37190]],0.975265871796</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:03.178049 Reading Data</t>
+  </si>
+  <si>
+    <t>((657532, 69), (657532,))</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:42.997456 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:42.997886 Training Random Forest classifier, [4, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:48.555768 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:49.843883 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.993281949269,[[244680, 1713], [1600, 245156]],0.999400044198</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:50.472889 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.992937225869,[[81778, 595], [566, 81444]],0.999381350922</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:51:55.213072 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.889535183354,[[2576355, 303343], [26742, 81706]],0.914083386045</t>
+  </si>
+  <si>
+    <t>day wise scores</t>
+  </si>
+  <si>
+    <t>(1041133, array([ 0.50998554]))</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:00.579069 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>5,Unseen,0.896306235611,[[903314, 98377], [9582, 29860]],0.919255452295</t>
+  </si>
+  <si>
+    <t>(696453, array([ 1.02805041]))</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:03.276621 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>4,Unseen,0.88496854777,[[592054, 72453], [7661, 24285]],0.915187115302</t>
+  </si>
+  <si>
+    <t>(1250560, array([ 1.54611528]))</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:07.063115 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>6,Unseen,0.886441274309,[[1080987, 132513], [9499, 27561]],0.90809917358</t>
+  </si>
+  <si>
+    <t>[  1.82878908e-03   1.50452271e-03   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.70635713e-04   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   8.53459247e-06   5.72022202e-05   4.64200583e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.09292064e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.29113973e-07   2.67161894e-03   0.00000000e+00   1.12398028e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.89041447e-03   2.95153469e-03   1.36223944e-03   4.08586916e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   7.07289814e-02   3.13490956e-04   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   2.16859603e-04   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   1.20629522e-08   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.75418844e-02   2.24519881e-03   0.00000000e+00   4.14876110e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.20325226e-01   1.28993224e-06   0.00000000e+00   5.18516147e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.56653123e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.06422359e-01   6.70291554e-03   6.07926844e-03   5.02164671e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.77728633e-02   7.48383994e-04   2.84602241e-02   4.89228332e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.18592490e-01   3.54802300e-07   0.00000000e+00   2.87864825e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.42245047e-03]</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:12.811246 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:14.100494 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.993137976555,[[244972, 1758], [1626, 244793]],0.999388585149</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:14.733151 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.993582061405,[[81468, 568], [487, 81860]],0.999408215419</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:19.496141 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.88959040154,[[2576504, 303194], [26726, 81722]],0.914365424048</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:24.844506 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>5,Unseen,0.896384995961,[[903389, 98302], [9575, 29867]],0.919487385447</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:27.560360 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>4,Unseen,0.885046083512,[[592102, 72405], [7655, 24291]],0.915608893959</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:31.328656 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>6,Unseen,0.88646446392,[[1081013, 132487], [9496, 27564]],0.908328397441</t>
+  </si>
+  <si>
+    <t>[  1.82044036e-03   1.49253937e-03   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.61419736e-04   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   2.15570454e-08   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   1.16727737e-05   1.02031440e-04   4.68137256e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.08193814e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   2.59880561e-03   0.00000000e+00   1.12419690e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.77925034e-03   2.88029838e-03   1.47973475e-03   3.96913064e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   7.13374918e-02   3.01679016e-04   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   1.68142167e-07   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.76304829e-02   2.17517599e-03   0.00000000e+00   4.17331028e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.20506927e-01   6.05026661e-06   0.00000000e+00   5.19319149e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.57636487e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.06628326e-01   6.95926973e-03   6.13467065e-03   5.60808153e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.79920573e-02   8.51917652e-04   2.82755328e-02   4.92065360e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.11183960e-01   1.25327612e-06   0.00000000e+00   2.89262310e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.45551671e-03]</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:37.410867 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:38.691866 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.993630728238,[[244850, 1629], [1512, 245158]],0.999395834255</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:39.324586 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.993235310221,[[81717, 570], [542, 81554]],0.999415227614</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:52:44.029177 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.904908260841,[[2616541, 263157], [20991, 87457]],0.924749895153</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:49.390436 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>5,Unseen,0.910318854556,[[915864, 85827], [7543, 31899]],0.92876838241</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:52.084688 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>4,Unseen,0.90195318277,[[602224, 62283], [6002, 25944]],0.926145593411</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:52:55.847821 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>6,Unseen,0.902049481832,[[1098453, 115047], [7446, 29614]],0.919712141082</t>
+  </si>
+  <si>
+    <t>[  0.00000000e+00   1.51230983e-03   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.18272603e-05   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   9.06158302e-06   7.90671301e-05   5.23343586e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.29125678e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   2.44852920e-04   0.00000000e+00   1.17192435e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.79096977e-03   1.49204813e-02   1.13326027e-03   1.92257724e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.68998473e-02   2.83034129e-04   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.75923736e-02   2.12081724e-03   1.06746626e-04   9.34191222e-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.78884348e-02   0.00000000e+00   0.00000000e+00   9.49111714e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.76268608e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.17559104e-01   6.98476461e-03   7.87225517e-03   5.64964294e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.56444262e-02   8.01619714e-04   2.84028226e-02   4.53373316e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.10496715e-01   4.06200938e-07   0.00000000e+00   7.14536728e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.34517984e-03]</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:53:01.733282 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:53:03.014915 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.993334671671,[[244920, 1776], [1511, 244942]],0.999377708595</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:53:03.655392 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.993381310719,[[81490, 580], [508, 81805]],0.999365006176</t>
+  </si>
+  <si>
+    <t>2017-08-09 07:53:08.343163 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.904701108982,[[2615826, 263872], [20895, 87553]],0.921453749269</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:53:13.716391 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>5,Unseen,0.910333261937,[[915840, 85851], [7504, 31938]],0.92652364315</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:53:16.426828 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>4,Unseen,0.900900706868,[[601472, 63035], [5983, 25963]],0.922413663045</t>
+  </si>
+  <si>
+    <t>day_ind, 2017-08-09 07:53:20.199974 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>6,Unseen,0.902128646366,[[1098514, 114986], [7408, 29652]],0.915637752886</t>
+  </si>
+  <si>
+    <t>[  0.00000000e+00   1.47040059e-03   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.59615634e-04   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   2.36031012e-03   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   1.17371256e-05   1.09605726e-04   5.45705239e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.29208610e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   2.77956238e-03   0.00000000e+00   1.11925144e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.79008794e-03   2.96713724e-03   8.27028999e-03   1.95189161e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.45754276e-02   3.38730065e-04   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.00000000e+00   0.00000000e+00   0.00000000e+00   2.63906370e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.94967534e-02   2.34292559e-03   0.00000000e+00   7.24507428e-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.96033817e-02   0.00000000e+00   7.53121651e-04   9.44537219e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.86712887e-02   0.00000000e+00   0.00000000e+00   0.00000000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.17910101e-01   6.97462611e-03   6.16662860e-03   5.63068806e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.54336428e-02   1.82184963e-06   2.86357460e-02   2.85306117e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.12829812e-01   1.52143723e-05   0.00000000e+00   8.76355178e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5.23904345e-03]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:13.571934 Reading Data</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:54.237427 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:54.237862 Training Random Forest classifier, [4, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:57.309866 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:58.088182 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.910659861421,[[221501, 25322], [18736, 227590]],0.970778220619</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:09:58.708821 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.909437107243,[[73453, 8490], [6397, 76043]],0.969767926277</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:03.113654 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.815018409408,[[2334746, 544952], [7800, 100648]],0.953149548146</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:08.652025 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:09.418868 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.911256030125,[[220498, 25760], [18004, 228887]],0.970917516125</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:10.038382 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.911846115474,[[73934, 8574], [5917, 75958]],0.971283369126</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:14.429412 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.809941013592,[[2319041, 560657], [7267, 101181]],0.954307961732</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:19.781884 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:20.552136 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.912746451884,[[222855, 23847], [19182, 227265]],0.970706389309</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:21.173796 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.913014119465,[[74096, 7968], [6331, 75988]],0.970659372585</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:25.566971 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.819544292682,[[2348618, 531080], [8148, 100300]],0.950883041101</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:31.065188 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:31.819944 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.910787611858,[[221274, 25241], [18754, 227880]],0.970628531613</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:32.438441 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.910538194339,[[73790, 8461], [6245, 75887]],0.971031406815</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:10:36.823241 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.813676105518,[[2330768, 548930], [7833, 100615]],0.952844009926</t>
+  </si>
+  <si>
+    <t>using top 15 features</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:14:08.510168 Reading Data</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:14:48.720398 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:14:48.720496 Training Logistic Regression classifier, [10, 'l2']</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:10.823178 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:11.516580 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.991181164313,[[244907, 1888], [2461, 243893]],0.999618620691</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:12.019454 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.991306886965,[[81326, 645], [784, 81628]],0.999620724642</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:12.914056 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.934782637796,[[2696250, 183448], [11431, 97017]],0.973316901461</t>
+  </si>
+  <si>
+    <t>[[ 0.07775114 -0.19136231 -0.22865681 -0.03243216  0.05247428 -0.63576688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.56497218  0.07384101  0.13574958  1.40699364  2.00669804 -3.02432462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.00433628  0.10675632  0.1245253  -0.34311692  0.03312837  0.13561743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.14441512 -0.09966443 -0.10448414 -0.11253718 -0.06818241 -1.49524649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.14848858 -0.28146499 -0.21748883 -1.59008563  2.62602709  0.08092001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.07366693  0.0876597   0.00303042 -0.11680417 -0.12130578  0.11889963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.22322964 -0.14798334 -0.17839946  0.4334659  -0.07383389  0.06019933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.06336303 -0.05339258 -0.13069806 -0.12873397 -0.23777787  0.57674453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.10989583  0.10365986  0.10771426  0.0322538   0.71789298 -0.07789773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.0803055   0.06072258  0.15158549  0.03819252  0.14120147 -0.26789264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.25714353  0.34483774  0.34907961  0.27602307  2.26941384 -0.04885209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.01503    -0.11279363  0.88981449]]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:41.962721 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:42.754699 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.991126414126,[[244733, 1919], [2457, 244040]],0.999614676969</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:43.247456 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.991312970319,[[81497, 617], [811, 81458]],0.999627975492</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:15:43.985827 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.933502245205,[[2692166, 187532], [11173, 97275]],0.973324220694</t>
+  </si>
+  <si>
+    <t>[[ 0.0443889  -0.17231995 -0.23489043 -0.01911882  0.05729109 -0.44208224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.4548424   0.01661562  0.19027545  1.40487809  1.98010701 -2.84779679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.14274415  0.10164719  0.11766167 -0.30380571  0.05900578  0.16764346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.17880258 -0.12934079 -0.1170026  -0.11778125 -0.07458974 -1.45180055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.06965158 -0.29332391 -0.2350098  -1.43396815  2.45284424  0.08884182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.07947637  0.11065126  0.02303446 -0.09147368 -0.09411878  0.05029053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.23675482 -0.15773551 -0.18857384  0.43209084 -0.05852661  0.04314882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.04520437 -0.03406454 -0.15695262 -0.08039407 -0.151592    0.38020489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.15332551  0.08931108  0.09165262  0.04807173  0.69360189 -0.09971594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.10192208  0.05357689  0.19359191  0.03706328  0.14393429 -0.28022643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.26996844  0.33864004  0.34261074  0.27422435  2.22997311 -0.05717287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.03731731 -0.08692027  0.9111139 ]]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:13.973692 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:14.763802 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.991428554048,[[244712, 1856], [2371, 244210]],0.999624946183</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:15.255958 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.990704634908,[[81511, 687], [841, 81344]],0.999596400096</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:15.993489 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.92964801586,[[2680095, 199603], [10619, 97829]],0.973219712098</t>
+  </si>
+  <si>
+    <t>[[ 0.06263099 -0.16607495 -0.2941042  -0.01778443  0.06148933 -0.55556643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.53380158  0.04479196  0.15686985  1.43887398  2.04773022 -3.06048473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.03075726  0.08232278  0.09697197 -0.28856366  0.04816046  0.14476547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.15446165 -0.11298627 -0.11698708 -0.10404431 -0.06021713 -1.48115443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.12598712 -0.29951895 -0.2384781  -1.50416786  2.52257421  0.10387561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.09650608  0.09258047 -0.0187646  -0.10854271 -0.11209469  0.07978097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.2329846  -0.08654766 -0.10435655  0.25389189  0.00390413  0.04854577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.05089884 -0.03912665 -0.13410858 -0.23599465 -0.40468101  0.85563695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.11902165  0.10210297  0.10504906  0.05021629  0.69360398 -0.09124693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.09389753  0.06644714  0.15428988  0.0356421   0.1353028  -0.26035525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.27169185  0.34486017  0.34854989  0.28500284  2.27484431 -0.04481649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.00970621 -0.11280537  0.88897931]]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:45.703444 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:46.496481 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.991144664189,[[244354, 1929], [2438, 244428]],0.999618703902</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:46.989371 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.99144680411,[[81885, 598], [808, 81092]],0.999618706645</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:16:47.731197 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.932337643475,[[2688592, 191106], [11079, 97369]],0.973376880557</t>
+  </si>
+  <si>
+    <t>[[  7.54586280e-02  -1.91336060e-01  -2.44654280e-01  -4.02087632e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7.92603771e-02  -6.22311274e-01   6.12971027e-01   2.59326341e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.50061215e-01   1.45000509e+00   2.05814484e+00  -3.04457140e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -6.21465643e-02   1.20326658e-01   1.40754714e-01  -3.96868731e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.48788638e-02   1.32593604e-01   1.40845736e-01  -8.98836517e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1.19263139e-01  -1.12654200e-01  -7.27679874e-02  -1.33869274e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.95780034e+00  -2.96767486e-01  -2.35333787e-01  -1.51580702e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.54642466e+00   9.11594415e-02   8.33641003e-02   9.48930524e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.80252958e-03  -1.00235527e-01  -1.03175021e-01   5.71033426e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.17444863e-01  -1.37223515e-01  -1.64735481e-01   3.88842404e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -5.95636827e-02   3.71942630e-02   3.93550174e-02  -3.70747078e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1.18575010e-01  -1.64855264e-01  -2.92163397e-01   6.58899806e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.21569832e-01   1.02533997e-01   1.06186730e-01   3.82020165e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.82461552e-01  -7.28131892e-02  -7.47677144e-02   4.85954883e-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.71192908e-01   4.18610139e-02   1.47275360e-01  -2.71665773e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.24441113e+00   3.46468052e-01   3.51203425e-01   2.69647337e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.29745428e+00  -4.99278769e-02  -1.85582477e-02  -1.07970410e-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8.95160001e-01]]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:07.904845 Reading Data</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:48.741513 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:48.741897 Training Random Forest classifier, [4, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:51.144487 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:51.828755 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.991057469446,[[242530, 4236], [174, 246209]],0.999267932679</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:52.396498 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.990765468449,[[80548, 1452], [66, 82317]],0.999310565272</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:21:56.393663 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.744448229772,[[2136581, 743117], [20509, 87939]],0.884685683838</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:01.256972 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:01.948516 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.991197386591,[[242418, 4138], [203, 246390]],0.99925174681</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:02.515774 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.99155022113,[[80888, 1322], [67, 82106]],0.999256299106</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:06.489902 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.744591797054,[[2136821, 742877], [20320, 88128]],0.895565500988</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:11.299213 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:11.987823 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.991156830897,[[242252, 4127], [234, 246536]],0.999308734552</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:12.554537 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.991525887713,[[81055, 1332], [61, 81935]],0.999308707194</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:16.533489 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.744568036502,[[2137000, 742698], [20570, 87878]],0.892764853384</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:21.312074 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:21.999500 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.991095997356,[[242373, 4224], [167, 246385]],0.99918982903</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:22.566886 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.990643801366,[[80688, 1481], [57, 82157]],0.999155037397</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:22:26.554176 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.744444883215,[[2136464, 743234], [20402, 88046]],0.884646799715</t>
+  </si>
+  <si>
+    <t>using first 15 features</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:25:30.576462 Reading Data</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:10.936911 Reading Data Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:10.937320 Training Random Forest classifier, [4, 10, 10, 10]</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:14.405200 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:15.353852 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Train,0.947683154584,[[232836, 13521], [12279, 234513]],0.986658527115</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:15.994432 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Test,0.94767707123,[[77985, 4424], [4177, 77797]],0.98626938921</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:20.473605 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>0,Unseen,0.901424495323,[[2608336, 271362], [23196, 85252]],0.952578686299</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:26.380031 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:27.321039 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Train,0.947967044443,[[233491, 13252], [12408, 233998]],0.986650047123</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:27.960814 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Test,0.947354653462,[[77539, 4484], [4170, 78190]],0.986634782079</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:32.642431 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>1,Unseen,0.902466947733,[[2611547, 268151], [23292, 85156]],0.952626094147</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:38.746169 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:39.686552 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Train,0.947634487751,[[233035, 13433], [12391, 234290]],0.98658839346</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:40.309649 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Test,0.948619991118,[[77836, 4462], [3984, 78101]],0.986961939557</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:44.757092 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>2,Unseen,0.901107241748,[[2607327, 272371], [23135, 85313]],0.952709314249</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:50.823754 Model Training Complete</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:51.765028 KF_Index,Train,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Train,0.946657095523,[[233825, 12905], [13401, 233018]],0.986340830595</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:52.387748 KF_Index,Test,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Test,0.946807151591,[[77775, 4261], [4483, 77864]],0.986254944515</t>
+  </si>
+  <si>
+    <t>2017-08-09 08:26:56.843038 KF_Index,Unseen,Accuracy,Confusion_Matrix,AUC</t>
+  </si>
+  <si>
+    <t>3,Unseen,0.906285034265,[[2623152, 256546], [23488, 84960]],0.954378012178</t>
+  </si>
+  <si>
+    <t>using first 33 features</t>
   </si>
 </sst>
 </file>
@@ -11095,7 +12011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -11792,4 +12708,1497 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J255"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="J7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="J11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>184</v>
+      </c>
+      <c r="J13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="J15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="J16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="J18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="J20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>192</v>
+      </c>
+      <c r="J21" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="J22" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="J23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>195</v>
+      </c>
+      <c r="J24" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>196</v>
+      </c>
+      <c r="J25" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>197</v>
+      </c>
+      <c r="J26" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>198</v>
+      </c>
+      <c r="J27" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>200</v>
+      </c>
+      <c r="J29" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>201</v>
+      </c>
+      <c r="J30" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>195</v>
+      </c>
+      <c r="J31" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>202</v>
+      </c>
+      <c r="J32" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>203</v>
+      </c>
+      <c r="J33" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>204</v>
+      </c>
+      <c r="J34" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>205</v>
+      </c>
+      <c r="J35" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>206</v>
+      </c>
+      <c r="J36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>208</v>
+      </c>
+      <c r="J38" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>209</v>
+      </c>
+      <c r="J39" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>210</v>
+      </c>
+      <c r="J40" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>211</v>
+      </c>
+      <c r="J41" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>213</v>
+      </c>
+      <c r="J43" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>214</v>
+      </c>
+      <c r="J44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>215</v>
+      </c>
+      <c r="J45" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>183</v>
+      </c>
+      <c r="J47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>184</v>
+      </c>
+      <c r="J48" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="J49" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>218</v>
+      </c>
+      <c r="J50" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>187</v>
+      </c>
+      <c r="J51" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="J52" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>220</v>
+      </c>
+      <c r="J53" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="J54" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>221</v>
+      </c>
+      <c r="J55" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>222</v>
+      </c>
+      <c r="J56" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>223</v>
+      </c>
+      <c r="J57" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>224</v>
+      </c>
+      <c r="J58" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>225</v>
+      </c>
+      <c r="J59" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>226</v>
+      </c>
+      <c r="J60" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>227</v>
+      </c>
+      <c r="J61" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>228</v>
+      </c>
+      <c r="J62" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>229</v>
+      </c>
+      <c r="J63" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>230</v>
+      </c>
+      <c r="J64" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>231</v>
+      </c>
+      <c r="J65" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+      <c r="J66" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>195</v>
+      </c>
+      <c r="J67" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>232</v>
+      </c>
+      <c r="J68" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>233</v>
+      </c>
+      <c r="J69" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>234</v>
+      </c>
+      <c r="J70" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>235</v>
+      </c>
+      <c r="J71" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>236</v>
+      </c>
+      <c r="J72" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>237</v>
+      </c>
+      <c r="J73" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>238</v>
+      </c>
+      <c r="J74" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>239</v>
+      </c>
+      <c r="J75" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>240</v>
+      </c>
+      <c r="J76" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>241</v>
+      </c>
+      <c r="J77" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>242</v>
+      </c>
+      <c r="J78" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>243</v>
+      </c>
+      <c r="J79" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>244</v>
+      </c>
+      <c r="J80" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>245</v>
+      </c>
+      <c r="J81" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>183</v>
+      </c>
+      <c r="J82" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>184</v>
+      </c>
+      <c r="J83" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>246</v>
+      </c>
+      <c r="J84" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="J85" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>187</v>
+      </c>
+      <c r="J86" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>